<commit_message>
feat: fixes on v1 and dataset northwind
</commit_message>
<xml_diff>
--- a/test/query_test_results.xlsx
+++ b/test/query_test_results.xlsx
@@ -446,18 +446,18 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>SELECT p.productid, p."Name", 
+          <t>SELECT p.productid, p.name, 
   SUM(sod.unitprice * sod.orderqty - sod.unitpricediscount) AS total_revenue
  FROM product p
  JOIN salesorderdetail sod ON p.productid = sod.productid
- GROUP BY p.productid, p."Name"
+ GROUP BY p.productid, p.name
  ORDER BY total_revenue DESC
  LIMIT 5;</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>['productid', 'Name', 'total_revenue']</t>
+          <t>['productid', 'name', 'total_revenue']</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -493,14 +493,14 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>SELECT pc.productcategoryid, pc."Name" AS categoryname,
+          <t>SELECT pc.productcategoryid, pc.name AS categoryname,
   AVG(p.standardcost) AS avg_cost,
   AVG(p.listprice) AS avg_price,
   AVG(p.listprice - p.standardcost) AS avg_diff
  FROM product p
  JOIN productsubcategory ps ON p.productsubcategoryid = ps.productsubcategoryid
  JOIN productcategory pc ON ps.productcategoryid = pc.productcategoryid
- GROUP BY pc.productcategoryid, pc."Name";</t>
+ GROUP BY pc.productcategoryid, pc.name;</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -518,17 +518,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>SELECT v.businessentityid, v."Name", AVG(pv.averageleadtime) AS avg_lead_time
+          <t>SELECT v.businessentityid, v.name, AVG(pv.averageleadtime) AS avg_lead_time
  FROM vendor v
  JOIN productvendor pv ON v.businessentityid = pv.businessentityid
- GROUP BY v.businessentityid, v."Name"
+ GROUP BY v.businessentityid, v.name
  ORDER BY avg_lead_time ASC
  LIMIT 3;</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>['businessentityid', 'Name', 'avg_lead_time']</t>
+          <t>['businessentityid', 'name', 'avg_lead_time']</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -541,7 +541,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>SELECT st.territoryid, st."Name",
+          <t>SELECT st.territoryid, st.name,
   ((st.salesytd - st.saleslastyear) / NULLIF(st.saleslastyear, 0)) * 100 AS difference_percent
  FROM salesterritory st
  WHERE ABS((st.salesytd - st.saleslastyear) / NULLIF(st.saleslastyear, 0)) * 100 &gt; 10;</t>
@@ -549,7 +549,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>['territoryid', 'Name', 'difference_percent']</t>
+          <t>['territoryid', 'name', 'difference_percent']</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -562,16 +562,16 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>SELECT pm.productmodelid, pm."Name", COUNT(DISTINCT pmpdc.productdescriptionid) AS description_count
+          <t>SELECT pm.productmodelid, pm.name, COUNT(DISTINCT pmpdc.productdescriptionid) AS description_count
  FROM productmodel pm
  JOIN productmodelproductdescriptionculture pmpdc ON pm.productmodelid = pmpdc.productmodelid
- GROUP BY pm.productmodelid, pm."Name"
+ GROUP BY pm.productmodelid, pm.name
  HAVING COUNT(DISTINCT pmpdc.productdescriptionid) &gt; 2;</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>['productmodelid', 'Name', 'description_count']</t>
+          <t>['productmodelid', 'name', 'description_count']</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -802,7 +802,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>SELECT p.productid, p."Name"
+          <t>SELECT p.productid, p.name
  FROM product p
  LEFT JOIN salesorderdetail sod ON p.productid = sod.productid
  LEFT JOIN productreview pr ON p.productid = pr.productid
@@ -812,7 +812,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>['productid', 'Name']</t>
+          <t>['productid', 'name']</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -901,7 +901,7 @@
       <c r="A21" t="inlineStr">
         <is>
           <t>SELECT status, folderflag, COUNT(*) AS total_docs
- FROM "Document"
+ FROM document
  GROUP BY status, folderflag;</t>
         </is>
       </c>
@@ -920,7 +920,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>SELECT s."Name" AS store_name, e.businessentityid AS employeeid, sp.bonus
+          <t>SELECT s.name AS store_name, e.businessentityid AS employeeid, sp.bonus
  FROM store s
  JOIN salesperson sp ON s.salespersonid = sp.businessentityid
  JOIN employee e ON sp.businessentityid = e.businessentityid
@@ -943,7 +943,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>SELECT p.productid, p."Name", p.weight, avg_group.avg_weight AS avg_group_weight
+          <t>SELECT p.productid, p.name, p.weight, avg_group.avg_weight AS avg_group_weight
  FROM product p
  JOIN (
   SELECT sizeunitmeasurecode, AVG(weight) AS avg_weight
@@ -956,7 +956,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>['productid', 'Name', 'weight', 'avg_group_weight']</t>
+          <t>['productid', 'name', 'weight', 'avg_group_weight']</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -969,19 +969,19 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>SELECT p.productid, p."Name",
+          <t>SELECT p.productid, p.name,
   STDDEV(pch.standardcost) AS cost_stddev,
   COUNT(*) AS record_count
 FROM product p
 JOIN productcosthistory pch ON p.productid = pch.productid
-GROUP BY p.productid, p."Name"
+GROUP BY p.productid, p.name
 ORDER BY cost_stddev DESC
 LIMIT 5;</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>['productid', 'Name', 'cost_stddev', 'record_count']</t>
+          <t>['productid', 'name', 'cost_stddev', 'record_count']</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -994,19 +994,19 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>SELECT p.productid, p."Name",
+          <t>SELECT p.productid, p.name,
   SUM(COALESCE(t.actualcost, 0)) + SUM(COALESCE(ta.actualcost, 0)) AS total_cost
 FROM product p
 LEFT JOIN transactionhistory t ON p.productid = t.productid
 LEFT JOIN transactionhistoryarchive ta ON p.productid = ta.productid
-GROUP BY p.productid, p."Name"
+GROUP BY p.productid, p.name
 ORDER BY total_cost DESC
 LIMIT 10;</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>['productid', 'Name', 'total_cost']</t>
+          <t>['productid', 'name', 'total_cost']</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1065,20 +1065,20 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>SELECT pm.productmodelid, pm."Name",
+          <t>SELECT pm.productmodelid, pm.name,
   AVG(pr.rating) AS avg_rating,
   COUNT(pr.productreviewid) AS total_reviews
 FROM productmodel pm
 JOIN product p ON pm.productmodelid = p.productmodelid
 JOIN productreview pr ON p.productid = pr.productid
-GROUP BY pm.productmodelid, pm."Name"
+GROUP BY pm.productmodelid, pm.name
 ORDER BY avg_rating DESC
 LIMIT 10;</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>['productmodelid', 'Name', 'avg_rating', 'total_reviews']</t>
+          <t>['productmodelid', 'name', 'avg_rating', 'total_reviews']</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1091,18 +1091,18 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>SELECT l.locationid, l."Name",
-  SUM(wr.actualcost) AS total_actual_cost
-FROM workorderrouting wr
-JOIN "Location" l ON wr.locationid = l.locationid
-GROUP BY l.locationid, l."Name"
-ORDER BY total_actual_cost DESC
+          <t>SELECT l.locationid, l.name,
+  SUM(wr.actualcost) AS total_actual_cost
+FROM workorderrouting wr
+JOIN location l ON wr.locationid = l.locationid
+GROUP BY l.locationid, l.name
+ORDER BY total_actual_cost DESC
 LIMIT 10;</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>['locationid', 'Name', 'total_actual_cost']</t>
+          <t>['locationid', 'name', 'total_actual_cost']</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1115,13 +1115,13 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>SELECT pc."Name" AS category_name,
-  AVG(pv.averageleadtime) AS avg_leadtime
-FROM product p
-JOIN productsubcategory ps ON p.productsubcategoryid = ps.productsubcategoryid
-JOIN productcategory pc ON ps.productcategoryid = pc.productcategoryid
-JOIN productvendor pv ON p.productid = pv.productid
-GROUP BY pc."Name"
+          <t>SELECT pc.name AS category_name,
+  AVG(pv.averageleadtime) AS avg_leadtime
+FROM product p
+JOIN productsubcategory ps ON p.productsubcategoryid = ps.productsubcategoryid
+JOIN productcategory pc ON ps.productcategoryid = pc.productcategoryid
+JOIN productvendor pv ON p.productid = pv.productid
+GROUP BY pc.name
 ORDER BY avg_leadtime DESC;</t>
         </is>
       </c>
@@ -1163,17 +1163,17 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>SELECT s.shipmethodid, s."Name",
-  COUNT(*) AS usage_count
-FROM salesorderheader soh
-JOIN shipmethod s ON soh.shipmethodid = s.shipmethodid
-GROUP BY s.shipmethodid, s."Name"
+          <t>SELECT s.shipmethodid, s.name,
+  COUNT(*) AS usage_count
+FROM salesorderheader soh
+JOIN shipmethod s ON soh.shipmethodid = s.shipmethodid
+GROUP BY s.shipmethodid, s.name
 ORDER BY usage_count DESC;</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>['shipmethodid', 'Name', 'usage_count']</t>
+          <t>['shipmethodid', 'name', 'usage_count']</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1186,16 +1186,16 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>SELECT pc."Name" AS category_name,
-  MIN(p.weight) AS min_weight,
-  MAX(p.weight) AS max_weight,
-  MAX(p.weight) - MIN(p.weight) AS weight_diff
-FROM product p
-JOIN productsubcategory ps ON p.productsubcategoryid = ps.productsubcategoryid
-JOIN productcategory pc ON ps.productcategoryid = pc.productcategoryid
-WHERE p.weight IS NOT NULL
-GROUP BY pc."Name"
-ORDER BY weight_diff DESC
+          <t>SELECT pc.name AS category_name,
+  MIN(p.weight) AS min_weight,
+  MAX(p.weight) AS max_weight,
+  MAX(p.weight) - MIN(p.weight) AS weight_diff
+FROM product p
+JOIN productsubcategory ps ON p.productsubcategoryid = ps.productsubcategoryid
+JOIN productcategory pc ON ps.productcategoryid = pc.productcategoryid
+WHERE p.weight IS NOT NULL
+GROUP BY pc.name
+ORDER BY weight_diff DESC
 LIMIT 5;</t>
         </is>
       </c>
@@ -1333,13 +1333,13 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>SELECT 
-  sm."Name" AS shipmethod_name,
-  COUNT(*) AS num_orders
-FROM salesorderheader soh
-JOIN shipmethod sm ON soh.shipmethodid = sm.shipmethodid
-WHERE soh.totaldue &gt; 5000
-GROUP BY sm."Name"
+          <t>SELECT 
+  sm.name AS shipmethod_name,
+  COUNT(*) AS num_orders
+FROM salesorderheader soh
+JOIN shipmethod sm ON soh.shipmethodid = sm.shipmethodid
+WHERE soh.totaldue &gt; 5000
+GROUP BY sm.name
 ORDER BY num_orders DESC;</t>
         </is>
       </c>
@@ -1545,11 +1545,11 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>SELECT edh.departmentid,
-       SUM(COALESCE(edh.enddate, CURRENT_DATE) - edh.startdate) AS total_days
-FROM employeedepartmenthistory edh
-GROUP BY edh.departmentid
-ORDER BY total_days DESC
+          <t>SELECT edh.departmentid,
+       SUM(COALESCE(edh.enddate, CURRENT_DATE) - edh.startdate) AS total_days
+FROM employeedepartmenthistory edh
+GROUP BY edh.departmentid
+ORDER BY total_days DESC
 LIMIT 5;</t>
         </is>
       </c>
@@ -1591,19 +1591,19 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>SELECT pc.productcategoryid, pc."Name", COUNT(DISTINCT sod.productid) AS product_count
+          <t>SELECT pc.productcategoryid, pc.name, COUNT(DISTINCT sod.productid) AS product_count
   FROM salesorderdetail sod
   JOIN product p ON sod.productid = p.productid
   JOIN productsubcategory ps ON p.productsubcategoryid = ps.productsubcategoryid
   JOIN productcategory pc ON ps.productcategoryid = pc.productcategoryid
-  GROUP BY pc.productcategoryid, pc."Name"
+  GROUP BY pc.productcategoryid, pc.name
   ORDER BY product_count DESC
   LIMIT 5;</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>['productcategoryid', 'Name', 'product_count']</t>
+          <t>['productcategoryid', 'name', 'product_count']</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">

</xml_diff>